<commit_message>
refactor(config.xlsx): expt_input_voltage -> expt_excitation_voltage
- CLI: read new column name; fallback to legacy if absent
- ThrustPostProcess __main__: support new column with legacy fallback
- Wire through call sites to use expt_excitation_voltage
</commit_message>
<xml_diff>
--- a/examples/config.xlsx
+++ b/examples/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr codeName="현재_통합_문서"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunseo/Documents/GitHub/static-fire-toolkit/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2795732D-5682-0A46-9B62-7B407A9B2752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94587CB-C7CD-624B-B561-101E75F76E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="16300" xr2:uid="{41B079AC-F165-4C68-9A00-B468E5ADFF0D}"/>
   </bookViews>
@@ -1050,10 +1050,6 @@
   </si>
   <si>
     <t>index</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>expt_input_voltage [V]</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -1094,6 +1090,10 @@
   </si>
   <si>
     <t>KNSB</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>expt_excitation_voltage [V]</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -2149,7 +2149,7 @@
     <tableColumn id="3" xr3:uid="{9D3B253A-1B39-BE49-ADC6-BB87C97742AA}" name="expt_file_name" dataDxfId="9" dataCellStyle="입력">
       <calculatedColumnFormula>표1[[#This Row],[type]] &amp; "_" &amp; 표1[[#This Row],[date]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{9E465FB0-BD64-FA41-8311-97F592CF5C12}" name="expt_input_voltage [V]" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{9E465FB0-BD64-FA41-8311-97F592CF5C12}" name="expt_excitation_voltage [V]" dataDxfId="8"/>
     <tableColumn id="5" xr3:uid="{3F351526-8E7E-7844-8074-5CB91144D465}" name="expt_resistance [Ohm]" dataDxfId="7"/>
     <tableColumn id="9" xr3:uid="{E27FAC17-833D-8541-9D7D-5DF887A591E9}" name="totalmass [g]" dataDxfId="6"/>
     <tableColumn id="11" xr3:uid="{876F3019-173B-194A-98B8-21E8A8A8030B}" name="Nozzlediameter [mm]" dataDxfId="5"/>
@@ -2493,7 +2493,7 @@
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="21" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.83203125" style="1" customWidth="1"/>
@@ -2512,37 +2512,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20" customHeight="1">
@@ -2553,7 +2553,7 @@
         <v>250220</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="str">
         <f>표1[[#This Row],[type]] &amp; "_" &amp; 표1[[#This Row],[date]]</f>
@@ -2584,7 +2584,7 @@
         <v>5</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="20" customHeight="1">

</xml_diff>